<commit_message>
Update Matriz de trazabilidad_Ordoñez_Rivas.xlsx
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{018D1DA6-B07C-48CC-9D63-5BB1022D7821}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A110B26F-AE7E-45AA-86A8-A292A5FBFB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
@@ -465,21 +465,25 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -676,6 +680,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -687,18 +703,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1016,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5:R6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,29 +1041,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="21" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="22" t="s">
+      <c r="L1" s="25"/>
+      <c r="M1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -1115,7 +1119,7 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1134,9 +1138,9 @@
         <v>125</v>
       </c>
       <c r="I3" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J3" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J3" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1162,7 +1166,7 @@
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1179,9 +1183,9 @@
         <v>125</v>
       </c>
       <c r="I4" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J4" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J4" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -1207,7 +1211,7 @@
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1224,9 +1228,9 @@
         <v>125</v>
       </c>
       <c r="I5" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J5" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J5" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1244,7 +1248,7 @@
       <c r="O5" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="25"/>
+      <c r="Q5" s="20"/>
     </row>
     <row r="6" spans="1:17" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -1253,7 +1257,7 @@
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="22"/>
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1270,9 +1274,9 @@
         <v>125</v>
       </c>
       <c r="I6" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J6" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1290,7 +1294,7 @@
       <c r="O6" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="Q6" s="25"/>
+      <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="1:17" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1299,7 +1303,7 @@
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1316,9 +1320,9 @@
         <v>125</v>
       </c>
       <c r="I7" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J7" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1344,7 +1348,7 @@
       <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="22"/>
       <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1361,9 +1365,9 @@
         <v>125</v>
       </c>
       <c r="I8" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J8" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J8" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1389,7 +1393,7 @@
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="22"/>
       <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
@@ -1406,9 +1410,9 @@
         <v>125</v>
       </c>
       <c r="I9" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J9" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1434,7 +1438,7 @@
       <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1451,9 +1455,9 @@
         <v>125</v>
       </c>
       <c r="I10" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J10" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1472,14 +1476,14 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1496,9 +1500,9 @@
         <v>125</v>
       </c>
       <c r="I11" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J11" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1524,7 +1528,7 @@
       <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="22"/>
       <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1541,9 +1545,9 @@
         <v>125</v>
       </c>
       <c r="I12" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J12" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1569,7 +1573,7 @@
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="22"/>
       <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
@@ -1586,9 +1590,9 @@
         <v>125</v>
       </c>
       <c r="I13" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J13" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1614,7 +1618,7 @@
       <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
@@ -1631,9 +1635,9 @@
         <v>125</v>
       </c>
       <c r="I14" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J14" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J14" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K14" s="8" t="s">
@@ -1659,7 +1663,7 @@
       <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
@@ -1676,9 +1680,9 @@
         <v>125</v>
       </c>
       <c r="I15" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J15" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K15" s="8" t="s">
@@ -1704,7 +1708,7 @@
       <c r="B16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="22" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1723,9 +1727,9 @@
         <v>25</v>
       </c>
       <c r="I16" s="12">
-        <v>43987</v>
-      </c>
-      <c r="J16" s="24" t="s">
+        <v>44109</v>
+      </c>
+      <c r="J16" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K16" s="8" t="s">
@@ -1751,7 +1755,7 @@
       <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="18"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1768,9 +1772,9 @@
         <v>25</v>
       </c>
       <c r="I17" s="12">
-        <v>43987</v>
-      </c>
-      <c r="J17" s="24" t="s">
+        <v>44109</v>
+      </c>
+      <c r="J17" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K17" s="8" t="s">
@@ -1796,7 +1800,7 @@
       <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="18"/>
+      <c r="C18" s="22"/>
       <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1813,9 +1817,9 @@
         <v>25</v>
       </c>
       <c r="I18" s="12">
-        <v>43990</v>
-      </c>
-      <c r="J18" s="24" t="s">
+        <v>44112</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K18" s="8" t="s">
@@ -1841,7 +1845,7 @@
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="18"/>
+      <c r="C19" s="22"/>
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1858,9 +1862,9 @@
         <v>25</v>
       </c>
       <c r="I19" s="12">
-        <v>43987</v>
-      </c>
-      <c r="J19" s="24" t="s">
+        <v>44109</v>
+      </c>
+      <c r="J19" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K19" s="8" t="s">
@@ -1886,7 +1890,7 @@
       <c r="B20" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="7" t="s">
         <v>129</v>
       </c>
@@ -1903,9 +1907,9 @@
         <v>125</v>
       </c>
       <c r="I20" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J20" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J20" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K20" s="8" t="s">
@@ -1931,7 +1935,7 @@
       <c r="B21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="22"/>
       <c r="D21" s="7" t="s">
         <v>130</v>
       </c>
@@ -1948,9 +1952,9 @@
         <v>125</v>
       </c>
       <c r="I21" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J21" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J21" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K21" s="8" t="s">
@@ -1976,7 +1980,7 @@
       <c r="B22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="22"/>
       <c r="D22" s="1" t="s">
         <v>74</v>
       </c>
@@ -1993,9 +1997,9 @@
         <v>25</v>
       </c>
       <c r="I22" s="12">
-        <v>43995</v>
-      </c>
-      <c r="J22" s="24" t="s">
+        <v>44117</v>
+      </c>
+      <c r="J22" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K22" s="8" t="s">
@@ -2021,7 +2025,7 @@
       <c r="B23" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="18"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="5" t="s">
         <v>41</v>
       </c>
@@ -2038,9 +2042,9 @@
         <v>25</v>
       </c>
       <c r="I23" s="12">
-        <v>43995</v>
-      </c>
-      <c r="J23" s="24" t="s">
+        <v>44117</v>
+      </c>
+      <c r="J23" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K23" s="8" t="s">
@@ -2066,7 +2070,7 @@
       <c r="B24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="18"/>
+      <c r="C24" s="22"/>
       <c r="D24" s="5" t="s">
         <v>79</v>
       </c>
@@ -2080,12 +2084,12 @@
         <v>24</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>125</v>
+        <v>25</v>
       </c>
       <c r="I24" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J24" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J24" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K24" s="8" t="s">
@@ -2111,7 +2115,7 @@
       <c r="B25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="18"/>
+      <c r="C25" s="22"/>
       <c r="D25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2128,9 +2132,9 @@
         <v>125</v>
       </c>
       <c r="I25" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J25" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J25" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K25" s="8" t="s">
@@ -2156,7 +2160,7 @@
       <c r="B26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="18"/>
+      <c r="C26" s="22"/>
       <c r="D26" s="5" t="s">
         <v>85</v>
       </c>
@@ -2173,9 +2177,9 @@
         <v>125</v>
       </c>
       <c r="I26" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J26" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J26" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K26" s="8" t="s">
@@ -2201,7 +2205,7 @@
       <c r="B27" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="18"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="5" t="s">
         <v>88</v>
       </c>
@@ -2218,9 +2222,9 @@
         <v>125</v>
       </c>
       <c r="I27" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J27" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J27" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K27" s="8" t="s">
@@ -2246,7 +2250,7 @@
       <c r="B28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="5" t="s">
         <v>91</v>
       </c>
@@ -2263,9 +2267,9 @@
         <v>125</v>
       </c>
       <c r="I28" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J28" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J28" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K28" s="8" t="s">
@@ -2291,7 +2295,7 @@
       <c r="B29" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="18"/>
+      <c r="C29" s="22"/>
       <c r="D29" s="5" t="s">
         <v>94</v>
       </c>
@@ -2308,7 +2312,7 @@
         <v>125</v>
       </c>
       <c r="I29" s="12">
-        <v>43994</v>
+        <v>44122</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>136</v>
@@ -2336,7 +2340,7 @@
       <c r="B30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="22"/>
       <c r="D30" s="5" t="s">
         <v>97</v>
       </c>
@@ -2353,9 +2357,9 @@
         <v>125</v>
       </c>
       <c r="I30" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J30" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J30" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K30" s="8" t="s">
@@ -2381,7 +2385,7 @@
       <c r="B31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="22" t="s">
         <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2400,9 +2404,9 @@
         <v>125</v>
       </c>
       <c r="I31" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J31" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J31" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K31" s="8" t="s">
@@ -2428,7 +2432,7 @@
       <c r="B32" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="18"/>
+      <c r="C32" s="22"/>
       <c r="D32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2445,9 +2449,9 @@
         <v>125</v>
       </c>
       <c r="I32" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J32" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J32" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K32" s="8" t="s">
@@ -2473,7 +2477,7 @@
       <c r="B33" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="18"/>
+      <c r="C33" s="22"/>
       <c r="D33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2490,9 +2494,9 @@
         <v>125</v>
       </c>
       <c r="I33" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J33" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J33" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K33" s="8" t="s">
@@ -2518,7 +2522,7 @@
       <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="18"/>
+      <c r="C34" s="22"/>
       <c r="D34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2535,9 +2539,9 @@
         <v>125</v>
       </c>
       <c r="I34" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J34" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J34" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K34" s="8" t="s">
@@ -2563,7 +2567,7 @@
       <c r="B35" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="22"/>
       <c r="D35" s="1" t="s">
         <v>105</v>
       </c>
@@ -2580,9 +2584,9 @@
         <v>125</v>
       </c>
       <c r="I35" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J35" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J35" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K35" s="8" t="s">
@@ -2608,7 +2612,7 @@
       <c r="B36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="18"/>
+      <c r="C36" s="22"/>
       <c r="D36" s="2" t="s">
         <v>97</v>
       </c>
@@ -2625,9 +2629,9 @@
         <v>125</v>
       </c>
       <c r="I36" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J36" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J36" s="19" t="s">
         <v>137</v>
       </c>
       <c r="K36" s="8" t="s">
@@ -2653,7 +2657,7 @@
       <c r="B37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="18"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="2" t="s">
         <v>110</v>
       </c>
@@ -2670,9 +2674,9 @@
         <v>125</v>
       </c>
       <c r="I37" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J37" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J37" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K37" s="8" t="s">
@@ -2698,7 +2702,7 @@
       <c r="B38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="18"/>
+      <c r="C38" s="22"/>
       <c r="D38" s="2" t="s">
         <v>134</v>
       </c>
@@ -2715,9 +2719,9 @@
         <v>125</v>
       </c>
       <c r="I38" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J38" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J38" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K38" s="8" t="s">
@@ -2740,10 +2744,10 @@
       <c r="A39" s="8">
         <v>37</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="18"/>
+      <c r="C39" s="22"/>
       <c r="D39" s="8" t="s">
         <v>113</v>
       </c>
@@ -2760,9 +2764,9 @@
         <v>125</v>
       </c>
       <c r="I39" s="12">
-        <v>43994</v>
-      </c>
-      <c r="J39" s="24" t="s">
+        <v>44122</v>
+      </c>
+      <c r="J39" s="19" t="s">
         <v>136</v>
       </c>
       <c r="K39" s="8" t="s">

</xml_diff>

<commit_message>
Gestionar Imagenes + Actualizacion Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A110B26F-AE7E-45AA-86A8-A292A5FBFB73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270655F0-87FB-4F8A-A7BA-0F44E967E40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
@@ -453,7 +453,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,8 +504,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +548,16 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -624,10 +648,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -655,9 +681,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -704,8 +727,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,74 +1072,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="25" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="21" t="s">
+      <c r="L1" s="24"/>
+      <c r="M1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1119,7 +1150,7 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1128,19 +1159,19 @@
       <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J3" s="19" t="s">
+      <c r="I3" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J3" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K3" s="1" t="s">
@@ -1149,13 +1180,13 @@
       <c r="L3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="M3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1166,26 +1197,26 @@
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I4" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J4" s="19" t="s">
+      <c r="I4" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J4" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K4" s="1" t="s">
@@ -1194,13 +1225,13 @@
       <c r="L4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="11" t="s">
+      <c r="M4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1211,26 +1242,26 @@
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J5" s="19" t="s">
+      <c r="I5" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J5" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -1239,16 +1270,16 @@
       <c r="L5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="11" t="s">
+      <c r="M5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="11" t="s">
+      <c r="O5" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="Q5" s="20"/>
+      <c r="Q5" s="19"/>
     </row>
     <row r="6" spans="1:17" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
@@ -1257,26 +1288,26 @@
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="21"/>
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J6" s="19" t="s">
+      <c r="I6" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K6" s="1" t="s">
@@ -1285,16 +1316,16 @@
       <c r="L6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M6" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" s="11" t="s">
+      <c r="M6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="11" t="s">
+      <c r="O6" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="Q6" s="20"/>
+      <c r="Q6" s="19"/>
     </row>
     <row r="7" spans="1:17" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -1303,26 +1334,26 @@
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J7" s="19" t="s">
+      <c r="I7" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J7" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K7" s="1" t="s">
@@ -1331,13 +1362,13 @@
       <c r="L7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="11" t="s">
+      <c r="M7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="11" t="s">
+      <c r="O7" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1348,26 +1379,26 @@
       <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J8" s="19" t="s">
+      <c r="I8" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J8" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K8" s="1" t="s">
@@ -1376,13 +1407,13 @@
       <c r="L8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="11" t="s">
+      <c r="M8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="11" t="s">
+      <c r="O8" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1393,26 +1424,26 @@
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I9" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J9" s="19" t="s">
+      <c r="I9" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J9" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1421,13 +1452,13 @@
       <c r="L9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="11" t="s">
+      <c r="M9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="11" t="s">
+      <c r="O9" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1438,26 +1469,26 @@
       <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J10" s="19" t="s">
+      <c r="I10" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J10" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K10" s="1" t="s">
@@ -1466,13 +1497,13 @@
       <c r="L10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" s="11" t="s">
+      <c r="M10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="11" t="s">
+      <c r="O10" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1483,26 +1514,26 @@
       <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I11" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J11" s="19" t="s">
+      <c r="I11" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J11" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K11" s="2" t="s">
@@ -1511,13 +1542,13 @@
       <c r="L11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="M11" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="11" t="s">
+      <c r="M11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="11" t="s">
+      <c r="O11" s="10" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1528,26 +1559,26 @@
       <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I12" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J12" s="19" t="s">
+      <c r="I12" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J12" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K12" s="2" t="s">
@@ -1556,13 +1587,13 @@
       <c r="L12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="11" t="s">
+      <c r="M12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="10" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1573,26 +1604,26 @@
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I13" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J13" s="19" t="s">
+      <c r="I13" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J13" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K13" s="2" t="s">
@@ -1601,13 +1632,13 @@
       <c r="L13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M13" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N13" s="11" t="s">
+      <c r="M13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="11" t="s">
+      <c r="O13" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1618,26 +1649,26 @@
       <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="21"/>
       <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I14" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J14" s="19" t="s">
+      <c r="I14" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K14" s="8" t="s">
@@ -1646,13 +1677,13 @@
       <c r="L14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N14" s="11" t="s">
+      <c r="M14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="11" t="s">
+      <c r="O14" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1663,26 +1694,26 @@
       <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="22"/>
+      <c r="C15" s="21"/>
       <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I15" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J15" s="19" t="s">
+      <c r="I15" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J15" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K15" s="8" t="s">
@@ -1691,13 +1722,13 @@
       <c r="L15" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M15" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N15" s="11" t="s">
+      <c r="M15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O15" s="10" t="s">
         <v>118</v>
       </c>
     </row>
@@ -1708,7 +1739,7 @@
       <c r="B16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="21" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1717,19 +1748,19 @@
       <c r="E16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="11">
         <v>44109</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K16" s="8" t="s">
@@ -1738,13 +1769,13 @@
       <c r="L16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N16" s="11" t="s">
+      <c r="M16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="O16" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1755,26 +1786,26 @@
       <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="11">
         <v>44109</v>
       </c>
-      <c r="J17" s="19" t="s">
+      <c r="J17" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K17" s="8" t="s">
@@ -1783,13 +1814,13 @@
       <c r="L17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N17" s="11" t="s">
+      <c r="M17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="O17" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1800,26 +1831,26 @@
       <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="21"/>
       <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="11">
         <v>44112</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K18" s="8" t="s">
@@ -1828,13 +1859,13 @@
       <c r="L18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M18" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N18" s="11" t="s">
+      <c r="M18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O18" s="11" t="s">
+      <c r="O18" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1845,26 +1876,26 @@
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="21"/>
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="11">
         <v>44109</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K19" s="8" t="s">
@@ -1873,13 +1904,13 @@
       <c r="L19" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" s="11" t="s">
+      <c r="M19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O19" s="11" t="s">
+      <c r="O19" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1890,26 +1921,26 @@
       <c r="B20" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="21"/>
       <c r="D20" s="7" t="s">
         <v>129</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I20" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J20" s="19" t="s">
+      <c r="I20" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J20" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K20" s="8" t="s">
@@ -1918,13 +1949,13 @@
       <c r="L20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M20" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N20" s="11" t="s">
+      <c r="M20" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1935,26 +1966,26 @@
       <c r="B21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="7" t="s">
         <v>130</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I21" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J21" s="19" t="s">
+      <c r="I21" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J21" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K21" s="8" t="s">
@@ -1963,13 +1994,13 @@
       <c r="L21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M21" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N21" s="11" t="s">
+      <c r="M21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O21" s="11" t="s">
+      <c r="O21" s="10" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1980,26 +2011,26 @@
       <c r="B22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="11">
         <v>44117</v>
       </c>
-      <c r="J22" s="19" t="s">
+      <c r="J22" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K22" s="8" t="s">
@@ -2008,13 +2039,13 @@
       <c r="L22" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N22" s="11" t="s">
+      <c r="M22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O22" s="11" t="s">
+      <c r="O22" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2025,26 +2056,26 @@
       <c r="B23" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="5" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F23" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="11">
         <v>44117</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K23" s="8" t="s">
@@ -2053,13 +2084,13 @@
       <c r="L23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M23" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N23" s="11" t="s">
+      <c r="M23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O23" s="11" t="s">
+      <c r="O23" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2070,26 +2101,26 @@
       <c r="B24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="5" t="s">
         <v>79</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="10" t="s">
+      <c r="H24" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="11">
         <v>44122</v>
       </c>
-      <c r="J24" s="19" t="s">
+      <c r="J24" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K24" s="8" t="s">
@@ -2098,13 +2129,13 @@
       <c r="L24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M24" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N24" s="11" t="s">
+      <c r="M24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O24" s="11" t="s">
+      <c r="O24" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2115,26 +2146,26 @@
       <c r="B25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="1" t="s">
         <v>82</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="I25" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J25" s="19" t="s">
+      <c r="H25" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J25" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K25" s="8" t="s">
@@ -2143,13 +2174,13 @@
       <c r="L25" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M25" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N25" s="11" t="s">
+      <c r="M25" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O25" s="11" t="s">
+      <c r="O25" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2160,26 +2191,26 @@
       <c r="B26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="21"/>
       <c r="D26" s="5" t="s">
         <v>85</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="11" t="s">
+      <c r="F26" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I26" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J26" s="19" t="s">
+      <c r="I26" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J26" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K26" s="8" t="s">
@@ -2188,13 +2219,13 @@
       <c r="L26" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M26" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N26" s="11" t="s">
+      <c r="M26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O26" s="11" t="s">
+      <c r="O26" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2205,26 +2236,26 @@
       <c r="B27" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="21"/>
       <c r="D27" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E27" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="11" t="s">
+      <c r="F27" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="10" t="s">
+      <c r="H27" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I27" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J27" s="19" t="s">
+      <c r="I27" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K27" s="8" t="s">
@@ -2233,13 +2264,13 @@
       <c r="L27" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M27" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N27" s="11" t="s">
+      <c r="M27" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O27" s="11" t="s">
+      <c r="O27" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2250,26 +2281,26 @@
       <c r="B28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="5" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F28" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="10" t="s">
+      <c r="H28" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I28" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J28" s="19" t="s">
+      <c r="I28" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J28" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K28" s="8" t="s">
@@ -2278,13 +2309,13 @@
       <c r="L28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M28" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N28" s="11" t="s">
+      <c r="M28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O28" s="11" t="s">
+      <c r="O28" s="10" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2295,24 +2326,24 @@
       <c r="B29" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="5" t="s">
         <v>94</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="11" t="s">
+      <c r="F29" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="10" t="s">
+      <c r="H29" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I29" s="12">
-        <v>44122</v>
+      <c r="I29" s="11">
+        <v>44127</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>136</v>
@@ -2323,13 +2354,13 @@
       <c r="L29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M29" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N29" s="11" t="s">
+      <c r="M29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O29" s="11" t="s">
+      <c r="O29" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2340,26 +2371,26 @@
       <c r="B30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="22"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F30" s="11" t="s">
+      <c r="F30" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="10" t="s">
+      <c r="H30" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I30" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J30" s="19" t="s">
+      <c r="I30" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J30" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K30" s="8" t="s">
@@ -2368,13 +2399,13 @@
       <c r="L30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M30" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N30" s="11" t="s">
+      <c r="M30" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O30" s="11" t="s">
+      <c r="O30" s="10" t="s">
         <v>120</v>
       </c>
     </row>
@@ -2385,7 +2416,7 @@
       <c r="B31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2394,19 +2425,19 @@
       <c r="E31" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="10" t="s">
+      <c r="H31" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I31" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J31" s="19" t="s">
+      <c r="I31" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J31" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K31" s="8" t="s">
@@ -2415,13 +2446,13 @@
       <c r="L31" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N31" s="11" t="s">
+      <c r="M31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O31" s="11" t="s">
+      <c r="O31" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2432,26 +2463,26 @@
       <c r="B32" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="22"/>
+      <c r="C32" s="21"/>
       <c r="D32" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="F32" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H32" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I32" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J32" s="19" t="s">
+      <c r="I32" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J32" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K32" s="8" t="s">
@@ -2460,13 +2491,13 @@
       <c r="L32" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M32" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N32" s="11" t="s">
+      <c r="M32" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O32" s="11" t="s">
+      <c r="O32" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2477,26 +2508,26 @@
       <c r="B33" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="21"/>
       <c r="D33" s="1" t="s">
         <v>34</v>
       </c>
       <c r="E33" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F33" s="11" t="s">
+      <c r="F33" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="H33" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I33" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J33" s="19" t="s">
+      <c r="I33" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J33" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K33" s="8" t="s">
@@ -2505,13 +2536,13 @@
       <c r="L33" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M33" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N33" s="11" t="s">
+      <c r="M33" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O33" s="11" t="s">
+      <c r="O33" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2522,26 +2553,26 @@
       <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="22"/>
+      <c r="C34" s="21"/>
       <c r="D34" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I34" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J34" s="19" t="s">
+      <c r="I34" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J34" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K34" s="8" t="s">
@@ -2550,13 +2581,13 @@
       <c r="L34" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N34" s="11" t="s">
+      <c r="M34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O34" s="11" t="s">
+      <c r="O34" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2567,26 +2598,26 @@
       <c r="B35" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="1" t="s">
         <v>105</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="10" t="s">
+      <c r="H35" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I35" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J35" s="19" t="s">
+      <c r="I35" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J35" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K35" s="8" t="s">
@@ -2595,13 +2626,13 @@
       <c r="L35" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M35" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N35" s="11" t="s">
+      <c r="M35" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O35" s="11" t="s">
+      <c r="O35" s="10" t="s">
         <v>123</v>
       </c>
     </row>
@@ -2612,26 +2643,26 @@
       <c r="B36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E36" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F36" s="11" t="s">
+      <c r="F36" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I36" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J36" s="19" t="s">
+      <c r="I36" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J36" s="18" t="s">
         <v>137</v>
       </c>
       <c r="K36" s="8" t="s">
@@ -2640,13 +2671,13 @@
       <c r="L36" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M36" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N36" s="11" t="s">
+      <c r="M36" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O36" s="11" t="s">
+      <c r="O36" s="10" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2657,26 +2688,26 @@
       <c r="B37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="2" t="s">
         <v>110</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I37" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J37" s="19" t="s">
+      <c r="I37" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J37" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K37" s="8" t="s">
@@ -2685,13 +2716,13 @@
       <c r="L37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M37" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N37" s="11" t="s">
+      <c r="M37" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N37" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O37" s="11" t="s">
+      <c r="O37" s="10" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2702,26 +2733,26 @@
       <c r="B38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="22"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="2" t="s">
         <v>134</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="F38" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="10" t="s">
+      <c r="H38" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I38" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J38" s="19" t="s">
+      <c r="I38" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J38" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K38" s="8" t="s">
@@ -2730,13 +2761,13 @@
       <c r="L38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M38" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N38" s="11" t="s">
+      <c r="M38" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N38" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O38" s="11" t="s">
+      <c r="O38" s="10" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2744,29 +2775,29 @@
       <c r="A39" s="8">
         <v>37</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="22"/>
+      <c r="C39" s="21"/>
       <c r="D39" s="8" t="s">
         <v>113</v>
       </c>
       <c r="E39" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F39" s="10" t="s">
         <v>23</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H39" s="10" t="s">
+      <c r="H39" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="I39" s="12">
-        <v>44122</v>
-      </c>
-      <c r="J39" s="19" t="s">
+      <c r="I39" s="11">
+        <v>44127</v>
+      </c>
+      <c r="J39" s="18" t="s">
         <v>136</v>
       </c>
       <c r="K39" s="8" t="s">
@@ -2775,13 +2806,13 @@
       <c r="L39" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="M39" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="N39" s="11" t="s">
+      <c r="M39" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N39" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="O39" s="11" t="s">
+      <c r="O39" s="10" t="s">
         <v>122</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gestionar Repartidor + Actualizacion Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270655F0-87FB-4F8A-A7BA-0F44E967E40D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD39C77-9B6C-4BB7-B2F3-A0B93839DEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
@@ -712,6 +712,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -725,12 +731,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26:H39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,29 +1072,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="24" t="s">
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="20" t="s">
+      <c r="L1" s="26"/>
+      <c r="M1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -1150,7 +1150,7 @@
       <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1165,7 +1165,7 @@
       <c r="G3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I3" s="11">
@@ -1197,7 +1197,7 @@
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I4" s="11">
@@ -1242,7 +1242,7 @@
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
@@ -1255,7 +1255,7 @@
       <c r="G5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I5" s="11">
@@ -1288,7 +1288,7 @@
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="G6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I6" s="11">
@@ -1334,7 +1334,7 @@
       <c r="B7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1347,7 +1347,7 @@
       <c r="G7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I7" s="11">
@@ -1379,7 +1379,7 @@
       <c r="B8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
@@ -1392,7 +1392,7 @@
       <c r="G8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I8" s="11">
@@ -1424,7 +1424,7 @@
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="G9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="26" t="s">
+      <c r="H9" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I9" s="11">
@@ -1469,7 +1469,7 @@
       <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1482,7 +1482,7 @@
       <c r="G10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="26" t="s">
+      <c r="H10" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I10" s="11">
@@ -1514,7 +1514,7 @@
       <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="2" t="s">
         <v>53</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="G11" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I11" s="11">
@@ -1559,7 +1559,7 @@
       <c r="B12" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="G12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I12" s="11">
@@ -1604,7 +1604,7 @@
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="21"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="2" t="s">
         <v>60</v>
       </c>
@@ -1617,7 +1617,7 @@
       <c r="G13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I13" s="11">
@@ -1649,7 +1649,7 @@
       <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="21"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="2" t="s">
         <v>62</v>
       </c>
@@ -1662,7 +1662,7 @@
       <c r="G14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I14" s="11">
@@ -1694,7 +1694,7 @@
       <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="2" t="s">
         <v>65</v>
       </c>
@@ -1707,7 +1707,7 @@
       <c r="G15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I15" s="11">
@@ -1739,7 +1739,7 @@
       <c r="B16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="23" t="s">
         <v>68</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1754,7 +1754,7 @@
       <c r="G16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I16" s="11">
@@ -1786,7 +1786,7 @@
       <c r="B17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="21"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1799,7 +1799,7 @@
       <c r="G17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I17" s="11">
@@ -1831,7 +1831,7 @@
       <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="21"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="1" t="s">
         <v>34</v>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="G18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="11">
@@ -1876,7 +1876,7 @@
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="21"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="1" t="s">
         <v>37</v>
       </c>
@@ -1889,7 +1889,7 @@
       <c r="G19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I19" s="11">
@@ -1921,7 +1921,7 @@
       <c r="B20" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="21"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="7" t="s">
         <v>129</v>
       </c>
@@ -1934,7 +1934,7 @@
       <c r="G20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="26" t="s">
+      <c r="H20" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I20" s="11">
@@ -1966,7 +1966,7 @@
       <c r="B21" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="7" t="s">
         <v>130</v>
       </c>
@@ -1979,7 +1979,7 @@
       <c r="G21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H21" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I21" s="11">
@@ -2011,7 +2011,7 @@
       <c r="B22" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="1" t="s">
         <v>74</v>
       </c>
@@ -2024,7 +2024,7 @@
       <c r="G22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="11">
@@ -2056,7 +2056,7 @@
       <c r="B23" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="5" t="s">
         <v>41</v>
       </c>
@@ -2069,7 +2069,7 @@
       <c r="G23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="11">
@@ -2101,7 +2101,7 @@
       <c r="B24" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="5" t="s">
         <v>79</v>
       </c>
@@ -2114,7 +2114,7 @@
       <c r="G24" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="25" t="s">
+      <c r="H24" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="11">
@@ -2146,7 +2146,7 @@
       <c r="B25" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="21"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="1" t="s">
         <v>82</v>
       </c>
@@ -2159,7 +2159,7 @@
       <c r="G25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="25" t="s">
+      <c r="H25" s="20" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="11">
@@ -2191,7 +2191,7 @@
       <c r="B26" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C26" s="21"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="5" t="s">
         <v>85</v>
       </c>
@@ -2204,7 +2204,7 @@
       <c r="G26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="26" t="s">
+      <c r="H26" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I26" s="11">
@@ -2236,7 +2236,7 @@
       <c r="B27" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="5" t="s">
         <v>88</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="G27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="26" t="s">
+      <c r="H27" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I27" s="11">
@@ -2281,7 +2281,7 @@
       <c r="B28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="5" t="s">
         <v>91</v>
       </c>
@@ -2294,7 +2294,7 @@
       <c r="G28" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H28" s="26" t="s">
+      <c r="H28" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I28" s="11">
@@ -2326,7 +2326,7 @@
       <c r="B29" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C29" s="21"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="5" t="s">
         <v>94</v>
       </c>
@@ -2339,8 +2339,8 @@
       <c r="G29" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="26" t="s">
-        <v>125</v>
+      <c r="H29" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I29" s="11">
         <v>44127</v>
@@ -2371,7 +2371,7 @@
       <c r="B30" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="23"/>
       <c r="D30" s="5" t="s">
         <v>97</v>
       </c>
@@ -2384,7 +2384,7 @@
       <c r="G30" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="26" t="s">
+      <c r="H30" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I30" s="11">
@@ -2416,7 +2416,7 @@
       <c r="B31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="23" t="s">
         <v>100</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -2431,7 +2431,7 @@
       <c r="G31" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="26" t="s">
+      <c r="H31" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I31" s="11">
@@ -2463,7 +2463,7 @@
       <c r="B32" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="21"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2476,7 +2476,7 @@
       <c r="G32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="26" t="s">
+      <c r="H32" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I32" s="11">
@@ -2508,7 +2508,7 @@
       <c r="B33" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C33" s="21"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="1" t="s">
         <v>34</v>
       </c>
@@ -2521,7 +2521,7 @@
       <c r="G33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="26" t="s">
+      <c r="H33" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I33" s="11">
@@ -2553,7 +2553,7 @@
       <c r="B34" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="21"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="1" t="s">
         <v>37</v>
       </c>
@@ -2566,7 +2566,7 @@
       <c r="G34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="26" t="s">
+      <c r="H34" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I34" s="11">
@@ -2598,7 +2598,7 @@
       <c r="B35" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="21"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="1" t="s">
         <v>105</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="G35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="26" t="s">
+      <c r="H35" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I35" s="11">
@@ -2643,7 +2643,7 @@
       <c r="B36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="21"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="2" t="s">
         <v>97</v>
       </c>
@@ -2656,7 +2656,7 @@
       <c r="G36" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="26" t="s">
+      <c r="H36" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I36" s="11">
@@ -2688,7 +2688,7 @@
       <c r="B37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="21"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="2" t="s">
         <v>110</v>
       </c>
@@ -2701,7 +2701,7 @@
       <c r="G37" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="26" t="s">
+      <c r="H37" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I37" s="11">
@@ -2733,7 +2733,7 @@
       <c r="B38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="21"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="2" t="s">
         <v>134</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="G38" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="26" t="s">
+      <c r="H38" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I38" s="11">
@@ -2778,7 +2778,7 @@
       <c r="B39" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="23"/>
       <c r="D39" s="8" t="s">
         <v>113</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="G39" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H39" s="26" t="s">
+      <c r="H39" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I39" s="11">

</xml_diff>

<commit_message>
Visualizar Resenas + Gestionar Menu + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD39C77-9B6C-4BB7-B2F3-A0B93839DEAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CF8FAA-EDCF-41E2-8D46-D0DB3BF9593A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
+    <workbookView xWindow="-25290" yWindow="345" windowWidth="21600" windowHeight="13470" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
         <v>125</v>
       </c>
       <c r="I3" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>137</v>
@@ -1214,7 +1214,7 @@
         <v>125</v>
       </c>
       <c r="I4" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>137</v>
@@ -1259,7 +1259,7 @@
         <v>125</v>
       </c>
       <c r="I5" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>137</v>
@@ -1305,7 +1305,7 @@
         <v>125</v>
       </c>
       <c r="I6" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>137</v>
@@ -1351,7 +1351,7 @@
         <v>125</v>
       </c>
       <c r="I7" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>136</v>
@@ -1396,7 +1396,7 @@
         <v>125</v>
       </c>
       <c r="I8" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>136</v>
@@ -1441,7 +1441,7 @@
         <v>125</v>
       </c>
       <c r="I9" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>137</v>
@@ -1486,7 +1486,7 @@
         <v>125</v>
       </c>
       <c r="I10" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>136</v>
@@ -1531,7 +1531,7 @@
         <v>125</v>
       </c>
       <c r="I11" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>136</v>
@@ -1576,7 +1576,7 @@
         <v>125</v>
       </c>
       <c r="I12" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>136</v>
@@ -1615,13 +1615,13 @@
         <v>23</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>24</v>
+        <v>55</v>
       </c>
       <c r="H13" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I13" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>136</v>
@@ -1666,7 +1666,7 @@
         <v>125</v>
       </c>
       <c r="I14" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>137</v>
@@ -1711,7 +1711,7 @@
         <v>125</v>
       </c>
       <c r="I15" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>136</v>
@@ -1938,7 +1938,7 @@
         <v>125</v>
       </c>
       <c r="I20" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>137</v>
@@ -1983,7 +1983,7 @@
         <v>125</v>
       </c>
       <c r="I21" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>137</v>
@@ -2204,11 +2204,11 @@
       <c r="G26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="21" t="s">
-        <v>125</v>
+      <c r="H26" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I26" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>136</v>
@@ -2249,11 +2249,11 @@
       <c r="G27" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="21" t="s">
-        <v>125</v>
+      <c r="H27" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I27" s="11">
-        <v>44127</v>
+        <v>44128</v>
       </c>
       <c r="J27" s="18" t="s">
         <v>136</v>
@@ -2292,13 +2292,13 @@
         <v>23</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="H28" s="21" t="s">
         <v>125</v>
       </c>
       <c r="I28" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J28" s="18" t="s">
         <v>137</v>
@@ -2388,7 +2388,7 @@
         <v>125</v>
       </c>
       <c r="I30" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>137</v>
@@ -2435,7 +2435,7 @@
         <v>125</v>
       </c>
       <c r="I31" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>137</v>
@@ -2480,7 +2480,7 @@
         <v>125</v>
       </c>
       <c r="I32" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J32" s="18" t="s">
         <v>137</v>
@@ -2525,7 +2525,7 @@
         <v>125</v>
       </c>
       <c r="I33" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J33" s="18" t="s">
         <v>137</v>
@@ -2570,7 +2570,7 @@
         <v>125</v>
       </c>
       <c r="I34" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J34" s="18" t="s">
         <v>137</v>
@@ -2615,7 +2615,7 @@
         <v>125</v>
       </c>
       <c r="I35" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>137</v>
@@ -2660,7 +2660,7 @@
         <v>125</v>
       </c>
       <c r="I36" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>137</v>
@@ -2705,7 +2705,7 @@
         <v>125</v>
       </c>
       <c r="I37" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J37" s="18" t="s">
         <v>136</v>
@@ -2750,7 +2750,7 @@
         <v>125</v>
       </c>
       <c r="I38" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J38" s="18" t="s">
         <v>136</v>
@@ -2795,7 +2795,7 @@
         <v>125</v>
       </c>
       <c r="I39" s="11">
-        <v>44127</v>
+        <v>44129</v>
       </c>
       <c r="J39" s="18" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Gestionar Vales + Actualizacion Matriz Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CF8FAA-EDCF-41E2-8D46-D0DB3BF9593A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE20F54A-47AB-496F-A297-3C4CF92299EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25290" yWindow="345" windowWidth="21600" windowHeight="13470" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
+    <workbookView xWindow="615" yWindow="1095" windowWidth="21600" windowHeight="13470" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,8 +2294,8 @@
       <c r="G28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="21" t="s">
-        <v>125</v>
+      <c r="H28" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I28" s="11">
         <v>44129</v>

</xml_diff>

<commit_message>
Configurar Metodo de Pago + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE20F54A-47AB-496F-A297-3C4CF92299EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5B279B-F390-414A-B846-24894DBCF9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="1095" windowWidth="21600" windowHeight="13470" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
         <v>125</v>
       </c>
       <c r="I3" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>137</v>
@@ -1214,7 +1214,7 @@
         <v>125</v>
       </c>
       <c r="I4" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>137</v>
@@ -1259,7 +1259,7 @@
         <v>125</v>
       </c>
       <c r="I5" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>137</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="126" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>125</v>
       </c>
       <c r="I6" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>137</v>
@@ -1351,7 +1351,7 @@
         <v>125</v>
       </c>
       <c r="I7" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>136</v>
@@ -1396,7 +1396,7 @@
         <v>125</v>
       </c>
       <c r="I8" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>136</v>
@@ -1441,7 +1441,7 @@
         <v>125</v>
       </c>
       <c r="I9" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>137</v>
@@ -1486,7 +1486,7 @@
         <v>125</v>
       </c>
       <c r="I10" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>136</v>
@@ -1531,7 +1531,7 @@
         <v>125</v>
       </c>
       <c r="I11" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>136</v>
@@ -1576,7 +1576,7 @@
         <v>125</v>
       </c>
       <c r="I12" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>136</v>
@@ -1621,7 +1621,7 @@
         <v>125</v>
       </c>
       <c r="I13" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>136</v>
@@ -1666,7 +1666,7 @@
         <v>125</v>
       </c>
       <c r="I14" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>137</v>
@@ -1711,7 +1711,7 @@
         <v>125</v>
       </c>
       <c r="I15" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>136</v>
@@ -1869,7 +1869,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="126" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -1934,11 +1934,11 @@
       <c r="G20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="21" t="s">
-        <v>125</v>
+      <c r="H20" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I20" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J20" s="18" t="s">
         <v>137</v>
@@ -1983,7 +1983,7 @@
         <v>125</v>
       </c>
       <c r="I21" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>137</v>
@@ -2004,7 +2004,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="126" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>125</v>
       </c>
       <c r="I30" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>137</v>
@@ -2435,7 +2435,7 @@
         <v>125</v>
       </c>
       <c r="I31" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>137</v>
@@ -2480,7 +2480,7 @@
         <v>125</v>
       </c>
       <c r="I32" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J32" s="18" t="s">
         <v>137</v>
@@ -2525,7 +2525,7 @@
         <v>125</v>
       </c>
       <c r="I33" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J33" s="18" t="s">
         <v>137</v>
@@ -2546,7 +2546,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="126" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>125</v>
       </c>
       <c r="I34" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J34" s="18" t="s">
         <v>137</v>
@@ -2615,7 +2615,7 @@
         <v>125</v>
       </c>
       <c r="I35" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>137</v>
@@ -2636,7 +2636,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>125</v>
       </c>
       <c r="I36" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>137</v>
@@ -2705,7 +2705,7 @@
         <v>125</v>
       </c>
       <c r="I37" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J37" s="18" t="s">
         <v>136</v>
@@ -2750,7 +2750,7 @@
         <v>125</v>
       </c>
       <c r="I38" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J38" s="18" t="s">
         <v>136</v>
@@ -2795,7 +2795,7 @@
         <v>125</v>
       </c>
       <c r="I39" s="11">
-        <v>44129</v>
+        <v>44131</v>
       </c>
       <c r="J39" s="18" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Visualizar Tablero de informacion + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C5B279B-F390-414A-B846-24894DBCF9A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F059DF-6E5B-4F55-A99A-A3DF67C4146B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8ADA147-0AAC-4B46-917B-3BA281F67BA4}"/>
   </bookViews>
@@ -1051,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D1B5CD-DCAF-4FF4-BD3D-0D9FB0D46F90}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,7 +1169,7 @@
         <v>125</v>
       </c>
       <c r="I3" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J3" s="18" t="s">
         <v>137</v>
@@ -1214,7 +1214,7 @@
         <v>125</v>
       </c>
       <c r="I4" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J4" s="18" t="s">
         <v>137</v>
@@ -1259,7 +1259,7 @@
         <v>125</v>
       </c>
       <c r="I5" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J5" s="18" t="s">
         <v>137</v>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="Q5" s="19"/>
     </row>
-    <row r="6" spans="1:17" ht="126" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>4</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>125</v>
       </c>
       <c r="I6" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J6" s="18" t="s">
         <v>137</v>
@@ -1351,7 +1351,7 @@
         <v>125</v>
       </c>
       <c r="I7" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>136</v>
@@ -1396,7 +1396,7 @@
         <v>125</v>
       </c>
       <c r="I8" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J8" s="18" t="s">
         <v>136</v>
@@ -1441,7 +1441,7 @@
         <v>125</v>
       </c>
       <c r="I9" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J9" s="18" t="s">
         <v>137</v>
@@ -1486,7 +1486,7 @@
         <v>125</v>
       </c>
       <c r="I10" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J10" s="18" t="s">
         <v>136</v>
@@ -1531,7 +1531,7 @@
         <v>125</v>
       </c>
       <c r="I11" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J11" s="18" t="s">
         <v>136</v>
@@ -1576,7 +1576,7 @@
         <v>125</v>
       </c>
       <c r="I12" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J12" s="18" t="s">
         <v>136</v>
@@ -1621,7 +1621,7 @@
         <v>125</v>
       </c>
       <c r="I13" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J13" s="18" t="s">
         <v>136</v>
@@ -1666,7 +1666,7 @@
         <v>125</v>
       </c>
       <c r="I14" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J14" s="18" t="s">
         <v>137</v>
@@ -1711,7 +1711,7 @@
         <v>125</v>
       </c>
       <c r="I15" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J15" s="18" t="s">
         <v>136</v>
@@ -1869,7 +1869,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="126" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
@@ -1979,11 +1979,11 @@
       <c r="G21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="21" t="s">
-        <v>125</v>
+      <c r="H21" s="20" t="s">
+        <v>25</v>
       </c>
       <c r="I21" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J21" s="18" t="s">
         <v>137</v>
@@ -2004,7 +2004,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="63" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="126" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -2388,7 +2388,7 @@
         <v>125</v>
       </c>
       <c r="I30" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J30" s="18" t="s">
         <v>137</v>
@@ -2435,7 +2435,7 @@
         <v>125</v>
       </c>
       <c r="I31" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J31" s="18" t="s">
         <v>137</v>
@@ -2480,7 +2480,7 @@
         <v>125</v>
       </c>
       <c r="I32" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J32" s="18" t="s">
         <v>137</v>
@@ -2525,7 +2525,7 @@
         <v>125</v>
       </c>
       <c r="I33" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J33" s="18" t="s">
         <v>137</v>
@@ -2546,7 +2546,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="126" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>125</v>
       </c>
       <c r="I34" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J34" s="18" t="s">
         <v>137</v>
@@ -2615,7 +2615,7 @@
         <v>125</v>
       </c>
       <c r="I35" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J35" s="18" t="s">
         <v>137</v>
@@ -2636,7 +2636,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>125</v>
       </c>
       <c r="I36" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J36" s="18" t="s">
         <v>137</v>
@@ -2705,7 +2705,7 @@
         <v>125</v>
       </c>
       <c r="I37" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J37" s="18" t="s">
         <v>136</v>
@@ -2750,7 +2750,7 @@
         <v>125</v>
       </c>
       <c r="I38" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J38" s="18" t="s">
         <v>136</v>
@@ -2795,7 +2795,7 @@
         <v>125</v>
       </c>
       <c r="I39" s="11">
-        <v>44131</v>
+        <v>44132</v>
       </c>
       <c r="J39" s="18" t="s">
         <v>136</v>

</xml_diff>

<commit_message>
Recuperar contraseña, Autenticar y Registrar Usuario Tacna F&D + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E78141F-F6CB-481D-AC7A-E092BB5CFA6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6007B53F-82FD-4EFB-842C-FEB3380A6EB3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -727,6 +727,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -735,15 +740,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -964,7 +964,7 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I30" sqref="I30:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -988,29 +988,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="26" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="27" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="24"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1066,7 +1066,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1081,11 +1081,11 @@
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>25</v>
+      <c r="H3" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I3" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>26</v>
@@ -1113,7 +1113,7 @@
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1126,11 +1126,11 @@
       <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10" t="s">
-        <v>25</v>
+      <c r="H4" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>26</v>
@@ -1158,7 +1158,7 @@
       <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="20"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>26</v>
@@ -1204,7 +1204,7 @@
       <c r="B6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7" t="s">
         <v>39</v>
       </c>
@@ -1217,11 +1217,11 @@
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>25</v>
+      <c r="H6" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I6" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>26</v>
@@ -1250,7 +1250,7 @@
       <c r="B7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="7" t="s">
         <v>43</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>45</v>
@@ -1295,7 +1295,7 @@
       <c r="B8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="20"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="14" t="s">
         <v>48</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>45</v>
@@ -1340,7 +1340,7 @@
       <c r="B9" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="14" t="s">
         <v>51</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>25</v>
       </c>
       <c r="I9" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>26</v>
@@ -1385,7 +1385,7 @@
       <c r="B10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="14" t="s">
         <v>54</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>45</v>
@@ -1430,7 +1430,7 @@
       <c r="B11" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="14" t="s">
         <v>57</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1475,7 +1475,7 @@
       <c r="B12" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="14" t="s">
         <v>62</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1520,7 +1520,7 @@
       <c r="B13" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="14" t="s">
         <v>65</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1565,7 +1565,7 @@
       <c r="B14" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="20"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="14" t="s">
         <v>69</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1610,7 +1610,7 @@
       <c r="B15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="21"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="14" t="s">
         <v>72</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -1655,7 +1655,7 @@
       <c r="B16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="22" t="s">
         <v>75</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1702,7 +1702,7 @@
       <c r="B17" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="20"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="7" t="s">
         <v>33</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="B18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="20"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="7" t="s">
         <v>36</v>
       </c>
@@ -1792,7 +1792,7 @@
       <c r="B19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="7" t="s">
         <v>39</v>
       </c>
@@ -1837,7 +1837,7 @@
       <c r="B20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="20"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="7" t="s">
         <v>83</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="B21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="20"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="7" t="s">
         <v>86</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="B22" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="20"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="7" t="s">
         <v>89</v>
       </c>
@@ -1972,7 +1972,7 @@
       <c r="B23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="18" t="s">
         <v>43</v>
       </c>
@@ -2017,7 +2017,7 @@
       <c r="B24" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="20"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="18" t="s">
         <v>95</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="B25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="20"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="7" t="s">
         <v>98</v>
       </c>
@@ -2107,7 +2107,7 @@
       <c r="B26" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="20"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="18" t="s">
         <v>101</v>
       </c>
@@ -2152,7 +2152,7 @@
       <c r="B27" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="20"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="18" t="s">
         <v>104</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="B28" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="20"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="18" t="s">
         <v>107</v>
       </c>
@@ -2242,7 +2242,7 @@
       <c r="B29" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="20"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="18" t="s">
         <v>111</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="B30" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="21"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="18" t="s">
         <v>114</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>25</v>
       </c>
       <c r="I30" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>26</v>
@@ -2332,7 +2332,7 @@
       <c r="B31" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="22" t="s">
         <v>117</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -2351,7 +2351,7 @@
         <v>25</v>
       </c>
       <c r="I31" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J31" s="12" t="s">
         <v>26</v>
@@ -2379,7 +2379,7 @@
       <c r="B32" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="20"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="7" t="s">
         <v>33</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>25</v>
       </c>
       <c r="I32" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J32" s="12" t="s">
         <v>26</v>
@@ -2424,7 +2424,7 @@
       <c r="B33" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C33" s="20"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="7" t="s">
         <v>36</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>25</v>
       </c>
       <c r="I33" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>26</v>
@@ -2469,7 +2469,7 @@
       <c r="B34" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="20"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="7" t="s">
         <v>39</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>25</v>
       </c>
       <c r="I34" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J34" s="12" t="s">
         <v>26</v>
@@ -2514,7 +2514,7 @@
       <c r="B35" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C35" s="20"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="7" t="s">
         <v>123</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2559,7 +2559,7 @@
       <c r="B36" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="20"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="14" t="s">
         <v>114</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2604,7 +2604,7 @@
       <c r="B37" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="C37" s="20"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="14" t="s">
         <v>130</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2649,7 +2649,7 @@
       <c r="B38" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="20"/>
+      <c r="C38" s="23"/>
       <c r="D38" s="14" t="s">
         <v>133</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2694,7 +2694,7 @@
       <c r="B39" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="21"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="6" t="s">
         <v>136</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44132</v>
+        <v>44135</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Modificar Usuario Repartidor + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{668CCCBD-BB91-4EB9-B378-2180D5DD53BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5604E2DD-3537-4D91-BFE3-962A9B7478B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1175,7 +1175,7 @@
         <v>25</v>
       </c>
       <c r="I5" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>26</v>
@@ -1267,7 +1267,7 @@
         <v>25</v>
       </c>
       <c r="I7" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>45</v>
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>45</v>
@@ -1357,7 +1357,7 @@
         <v>25</v>
       </c>
       <c r="I9" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>26</v>
@@ -1402,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>45</v>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2437,11 +2437,11 @@
       <c r="G33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>25</v>
+      <c r="H33" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I33" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>26</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44135</v>
+        <v>44136</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Buscar Establecimiento Tacna F&D + Actualizacion Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5604E2DD-3537-4D91-BFE3-962A9B7478B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0E41D-AB6F-4EEA-867C-5FA96C4FF978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1171,11 +1171,11 @@
       <c r="G5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="10" t="s">
-        <v>25</v>
+      <c r="H5" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I5" s="11">
-        <v>44136</v>
+        <v>44140</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>26</v>
@@ -1263,11 +1263,11 @@
       <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>25</v>
+      <c r="H7" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I7" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>45</v>
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>45</v>
@@ -1357,7 +1357,7 @@
         <v>25</v>
       </c>
       <c r="I9" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>26</v>
@@ -1402,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="I10" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>45</v>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2304,7 +2304,7 @@
         <v>25</v>
       </c>
       <c r="I30" s="11">
-        <v>44135</v>
+        <v>44143</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>26</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44136</v>
+        <v>44143</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Listar Menu + Actualizacion Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0E41D-AB6F-4EEA-867C-5FA96C4FF978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49203673-1F17-4CEC-B63D-AD070BC6EBD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4545" yWindow="1380" windowWidth="21600" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1288,7 +1288,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>25</v>
       </c>
       <c r="I8" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>45</v>
@@ -1357,7 +1357,7 @@
         <v>25</v>
       </c>
       <c r="I9" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>26</v>
@@ -1398,11 +1398,11 @@
       <c r="G10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="10" t="s">
-        <v>25</v>
+      <c r="H10" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I10" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>45</v>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2304,7 +2304,7 @@
         <v>25</v>
       </c>
       <c r="I30" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J30" s="12" t="s">
         <v>26</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44143</v>
+        <v>44146</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Listar Pedido + Actualizacion de Matriz de Trazabilidad y docucumentos
Se Completo el requerimiento Listar Pedidos, Ademas de actualizar la Matriz de trazabilidad y documentos relacionados con el requerimiento debido a la agregacion de nuevos estados del pedido.
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademuz\Documents\GitHub\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49203673-1F17-4CEC-B63D-AD070BC6EBD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A288F896-56B6-4D2E-8750-3D4B13E91CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="1380" windowWidth="21600" windowHeight="13470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -372,9 +372,6 @@
     <t>Listar Pedidos</t>
   </si>
   <si>
-    <t>La aplicación debe permitir que el usuario pueda visualizar todos los pedidos (culminados o pendientes) realizados por los clientes</t>
-  </si>
-  <si>
     <t>RF-29</t>
   </si>
   <si>
@@ -439,6 +436,9 @@
   </si>
   <si>
     <t>La aplicación debe mostrar al usuario la ruta a seguir para llegar al cliente y actualizara su posición actual en la base de datos cada 7 segundos</t>
+  </si>
+  <si>
+    <t>La aplicación debe permitir que el usuario pueda visualizar todos los pedidos (pendiente, en camino, entregado o separado) realizados por los clientes</t>
   </si>
 </sst>
 </file>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2292,7 +2292,7 @@
         <v>114</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>23</v>
@@ -2300,8 +2300,8 @@
       <c r="G30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="10" t="s">
-        <v>25</v>
+      <c r="H30" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I30" s="11">
         <v>44146</v>
@@ -2330,10 +2330,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>117</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
@@ -2369,7 +2369,7 @@
         <v>77</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2377,7 +2377,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C32" s="23"/>
       <c r="D32" s="7" t="s">
@@ -2414,7 +2414,7 @@
         <v>77</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2422,7 +2422,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C33" s="23"/>
       <c r="D33" s="7" t="s">
@@ -2459,7 +2459,7 @@
         <v>77</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2467,7 +2467,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="23"/>
       <c r="D34" s="7" t="s">
@@ -2504,7 +2504,7 @@
         <v>77</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2512,14 +2512,14 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C35" s="23"/>
       <c r="D35" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>123</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>124</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>23</v>
@@ -2549,7 +2549,7 @@
         <v>77</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2557,14 +2557,14 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="14" t="s">
         <v>114</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>23</v>
@@ -2594,7 +2594,7 @@
         <v>77</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2602,14 +2602,14 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C37" s="23"/>
       <c r="D37" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>130</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>131</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>23</v>
@@ -2639,7 +2639,7 @@
         <v>77</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2647,14 +2647,14 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C38" s="23"/>
       <c r="D38" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>133</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>134</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>23</v>
@@ -2684,7 +2684,7 @@
         <v>77</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2692,14 +2692,14 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="16" t="s">
         <v>136</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>137</v>
       </c>
       <c r="F39" s="9" t="s">
         <v>23</v>
@@ -2729,7 +2729,7 @@
         <v>77</v>
       </c>
       <c r="O39" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Gestionar Reseña + Actualizacion Matriz de Trazabilidad + Estructura del Plan de gestion de riesgos
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademuz\Documents\GitHub\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A288F896-56B6-4D2E-8750-3D4B13E91CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C9FAF7-9CF2-4F43-98D2-7AEE5D26CB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1308,11 +1308,11 @@
       <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>25</v>
+      <c r="H8" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I8" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>45</v>
@@ -1353,11 +1353,11 @@
       <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>25</v>
+      <c r="H9" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I9" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>26</v>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1537,7 +1537,7 @@
         <v>25</v>
       </c>
       <c r="I13" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1582,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="I14" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44146</v>
+        <v>44147</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Realizar Pedido + Actualizar Matriz de Trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C9FAF7-9CF2-4F43-98D2-7AEE5D26CB70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1ECD06-C197-41AF-8C3F-363CCE91CEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1447,7 +1447,7 @@
         <v>25</v>
       </c>
       <c r="I11" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1492,7 +1492,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1533,11 +1533,11 @@
       <c r="G13" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>25</v>
+      <c r="H13" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I13" s="11">
-        <v>44147</v>
+        <v>44152</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>45</v>
@@ -1578,11 +1578,11 @@
       <c r="G14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>25</v>
+      <c r="H14" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I14" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44147</v>
+        <v>44153</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Obtener Vale + Listar Vale + Actualizacion Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1ECD06-C197-41AF-8C3F-363CCE91CEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156471F7-E98D-4C7A-AEFB-A8FDE610182B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1443,11 +1443,11 @@
       <c r="G11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>25</v>
+      <c r="H11" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I11" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>45</v>
@@ -1488,11 +1488,11 @@
       <c r="G12" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H12" s="10" t="s">
-        <v>25</v>
+      <c r="H12" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I12" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>45</v>
@@ -1627,7 +1627,7 @@
         <v>25</v>
       </c>
       <c r="I15" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J15" s="12" t="s">
         <v>45</v>
@@ -2531,7 +2531,7 @@
         <v>25</v>
       </c>
       <c r="I35" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2576,7 +2576,7 @@
         <v>25</v>
       </c>
       <c r="I36" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2621,7 +2621,7 @@
         <v>25</v>
       </c>
       <c r="I37" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J37" s="12" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>25</v>
       </c>
       <c r="I38" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J38" s="12" t="s">
         <v>45</v>
@@ -2711,7 +2711,7 @@
         <v>25</v>
       </c>
       <c r="I39" s="11">
-        <v>44153</v>
+        <v>44155</v>
       </c>
       <c r="J39" s="12" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Listar_Establecimiento + Listar_Pedido + Actualizacion Documentos
Completado requerimiento
Listar Establecimiento
Listar_Pedido
Actualizacion Matriz trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademuz\Documents\GitHub\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156471F7-E98D-4C7A-AEFB-A8FDE610182B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7F348-F9D6-4671-BA84-1CE9099754FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="135">
   <si>
     <t>IDENTIFICACION</t>
   </si>
@@ -421,15 +421,6 @@
   </si>
   <si>
     <t>RF-36</t>
-  </si>
-  <si>
-    <t>Separar Pedido</t>
-  </si>
-  <si>
-    <t>La aplicación debe permitir al usuario separar solo un pedido y no más de uno para poder realizar el seguimiento</t>
-  </si>
-  <si>
-    <t>RF-37</t>
   </si>
   <si>
     <t>Realizar Seguimiento del Pedido</t>
@@ -961,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q1000"/>
+  <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2292,7 +2283,7 @@
         <v>114</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>23</v>
@@ -2527,11 +2518,11 @@
       <c r="G35" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>25</v>
+      <c r="H35" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I35" s="11">
-        <v>44155</v>
+        <v>44160</v>
       </c>
       <c r="J35" s="12" t="s">
         <v>26</v>
@@ -2572,11 +2563,11 @@
       <c r="G36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="10" t="s">
-        <v>25</v>
+      <c r="H36" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="I36" s="11">
-        <v>44155</v>
+        <v>44160</v>
       </c>
       <c r="J36" s="12" t="s">
         <v>26</v>
@@ -2642,18 +2633,18 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="14" t="s">
+      <c r="C38" s="24"/>
+      <c r="D38" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="16" t="s">
         <v>133</v>
       </c>
       <c r="F38" s="9" t="s">
@@ -2675,7 +2666,7 @@
         <v>27</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>29</v>
@@ -2687,51 +2678,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6">
-        <v>37</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I39" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J39" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M39" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="O39" s="9" t="s">
-        <v>127</v>
-      </c>
-    </row>
+    <row r="39" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3692,13 +3639,12 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="M1:O1"/>
     <mergeCell ref="C3:C15"/>
     <mergeCell ref="C16:C30"/>
-    <mergeCell ref="C31:C39"/>
+    <mergeCell ref="C31:C38"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="K1:L1"/>

</xml_diff>

<commit_message>
Tacna FyD Delivery: Detalle Pedido, Seguimiento Pedido + Tacna FyD: Seguimiento Pedido + Actualizacion Matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademuz\Documents\GitHub\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E7F348-F9D6-4671-BA84-1CE9099754FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46D1A3-5CC6-4610-86E3-D47725026900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,9 +102,6 @@
     <t>v1</t>
   </si>
   <si>
-    <t>Falta</t>
-  </si>
-  <si>
     <t>Ronald Ordoñez Quilli</t>
   </si>
   <si>
@@ -430,6 +427,9 @@
   </si>
   <si>
     <t>La aplicación debe permitir que el usuario pueda visualizar todos los pedidos (pendiente, en camino, entregado o separado) realizados por los clientes</t>
+  </si>
+  <si>
+    <t>En Proceso</t>
   </si>
 </sst>
 </file>
@@ -457,11 +457,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -480,6 +475,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -515,14 +517,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -659,8 +660,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -691,9 +693,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -703,19 +702,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -737,8 +736,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -954,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -979,29 +982,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="27" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="21"/>
-      <c r="M1" s="19" t="s">
+      <c r="L1" s="20"/>
+      <c r="M1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="20"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1057,7 +1060,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1072,29 +1075,29 @@
       <c r="G3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I3" s="11">
+      <c r="H3" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I3" s="10">
         <v>44135</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>26</v>
+      <c r="J3" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1102,14 +1105,14 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>33</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>34</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>23</v>
@@ -1117,29 +1120,29 @@
       <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I4" s="11">
+      <c r="H4" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" s="10">
         <v>44135</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>26</v>
+      <c r="J4" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="M4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="O4" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="O4" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1147,14 +1150,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>36</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>37</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>23</v>
@@ -1162,45 +1165,45 @@
       <c r="G5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I5" s="11">
+      <c r="H5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" s="10">
         <v>44140</v>
       </c>
-      <c r="J5" s="12" t="s">
-        <v>26</v>
+      <c r="J5" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q5" s="13"/>
+      <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="1:17" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>23</v>
@@ -1208,45 +1211,45 @@
       <c r="G6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="11">
+      <c r="H6" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I6" s="10">
         <v>44135</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>26</v>
+      <c r="J6" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="O6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="13"/>
+      <c r="Q6" s="12"/>
     </row>
     <row r="7" spans="1:17" ht="138" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>23</v>
@@ -1254,29 +1257,29 @@
       <c r="G7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="11">
+      <c r="H7" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="10">
         <v>44143</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1284,14 +1287,14 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>23</v>
@@ -1299,29 +1302,29 @@
       <c r="G8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I8" s="11">
+      <c r="H8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="10">
         <v>44147</v>
       </c>
-      <c r="J8" s="12" t="s">
+      <c r="J8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1329,14 +1332,14 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="14" t="s">
+      <c r="E9" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>52</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>23</v>
@@ -1344,29 +1347,29 @@
       <c r="G9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I9" s="11">
+      <c r="H9" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" s="10">
         <v>44147</v>
       </c>
-      <c r="J9" s="12" t="s">
-        <v>26</v>
+      <c r="J9" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="7" t="s">
+      <c r="M9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N9" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="O9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1374,14 +1377,14 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>55</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>23</v>
@@ -1389,29 +1392,29 @@
       <c r="G10" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="10">
         <v>44146</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="J10" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1419,44 +1422,44 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>58</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="10">
+        <v>44155</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O11" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1464,44 +1467,44 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="14" t="s">
+      <c r="E12" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>63</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="10">
+        <v>44155</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="228" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,44 +1512,44 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="14" t="s">
+      <c r="E13" s="14" t="s">
         <v>65</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="11">
+        <v>58</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="10">
         <v>44152</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>27</v>
+      <c r="J13" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N13" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="O13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1554,14 +1557,14 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>70</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>23</v>
@@ -1569,29 +1572,29 @@
       <c r="G14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="11">
+      <c r="H14" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="10">
         <v>44153</v>
       </c>
-      <c r="J14" s="12" t="s">
-        <v>26</v>
+      <c r="J14" s="11" t="s">
+        <v>25</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M14" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="O14" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1599,14 +1602,14 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>73</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>23</v>
@@ -1614,29 +1617,29 @@
       <c r="G15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J15" s="12" t="s">
-        <v>45</v>
+      <c r="H15" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="10">
+        <v>44160</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N15" s="9" t="s">
-        <v>30</v>
-      </c>
       <c r="O15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -1644,15 +1647,15 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>75</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="9" t="s">
@@ -1661,29 +1664,29 @@
       <c r="G16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="10">
+        <v>44109</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I16" s="11">
-        <v>44109</v>
-      </c>
-      <c r="J16" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="9" t="s">
+      <c r="O16" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O16" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1691,14 +1694,14 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="23"/>
+        <v>78</v>
+      </c>
+      <c r="C17" s="22"/>
       <c r="D17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="F17" s="9" t="s">
         <v>23</v>
@@ -1706,29 +1709,29 @@
       <c r="G17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I17" s="10">
+        <v>44109</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I17" s="11">
-        <v>44109</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="9" t="s">
+      <c r="O17" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O17" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1736,14 +1739,14 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="23"/>
+        <v>79</v>
+      </c>
+      <c r="C18" s="22"/>
       <c r="D18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>37</v>
       </c>
       <c r="F18" s="9" t="s">
         <v>23</v>
@@ -1751,29 +1754,29 @@
       <c r="G18" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I18" s="10">
+        <v>44112</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="11">
-        <v>44112</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M18" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="9" t="s">
+      <c r="O18" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O18" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="132" customHeight="1" x14ac:dyDescent="0.2">
@@ -1781,14 +1784,14 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="23"/>
+        <v>80</v>
+      </c>
+      <c r="C19" s="22"/>
       <c r="D19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="F19" s="9" t="s">
         <v>23</v>
@@ -1796,29 +1799,29 @@
       <c r="G19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="10">
+        <v>44109</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I19" s="11">
-        <v>44109</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="9" t="s">
+      <c r="O19" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O19" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="165" customHeight="1" x14ac:dyDescent="0.2">
@@ -1826,14 +1829,14 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>23</v>
@@ -1841,29 +1844,29 @@
       <c r="G20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" s="10">
+        <v>44131</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="11">
-        <v>44131</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="9" t="s">
+      <c r="O20" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O20" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="257.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1871,14 +1874,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="7" t="s">
+      <c r="E21" s="14" t="s">
         <v>86</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>87</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>23</v>
@@ -1886,29 +1889,29 @@
       <c r="G21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="10">
+        <v>44132</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="11">
-        <v>44132</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K21" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="9" t="s">
+      <c r="O21" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="O21" s="9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1916,14 +1919,14 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="7" t="s">
+      <c r="E22" s="14" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>90</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>23</v>
@@ -1931,29 +1934,29 @@
       <c r="G22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" s="10">
+        <v>44117</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="11">
-        <v>44117</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O22" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1961,14 +1964,14 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>92</v>
-      </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>23</v>
@@ -1976,29 +1979,29 @@
       <c r="G23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="10">
+        <v>44117</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M23" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I23" s="11">
-        <v>44117</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O23" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2006,14 +2009,14 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="18" t="s">
+      <c r="E24" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>23</v>
@@ -2021,29 +2024,29 @@
       <c r="G24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I24" s="10">
+        <v>44122</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I24" s="11">
-        <v>44122</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M24" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O24" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2051,14 +2054,14 @@
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="7" t="s">
+      <c r="E25" s="14" t="s">
         <v>98</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>99</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>23</v>
@@ -2066,29 +2069,29 @@
       <c r="G25" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="10">
+        <v>44127</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I25" s="11">
-        <v>44127</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M25" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O25" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="171" customHeight="1" x14ac:dyDescent="0.2">
@@ -2096,14 +2099,14 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="18" t="s">
+      <c r="E26" s="14" t="s">
         <v>101</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>102</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>23</v>
@@ -2111,29 +2114,29 @@
       <c r="G26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="10">
+        <v>44129</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I26" s="11">
-        <v>44129</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M26" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N26" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O26" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2141,14 +2144,14 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>23</v>
@@ -2156,29 +2159,29 @@
       <c r="G27" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="10">
+        <v>44128</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N27" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I27" s="11">
-        <v>44128</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K27" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M27" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N27" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O27" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.2">
@@ -2186,14 +2189,14 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="18" t="s">
+      <c r="E28" s="14" t="s">
         <v>107</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>108</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>23</v>
@@ -2201,29 +2204,29 @@
       <c r="G28" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" s="10">
+        <v>44129</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I28" s="11">
-        <v>44129</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M28" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N28" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O28" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2231,14 +2234,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="18" t="s">
+      <c r="E29" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>112</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>23</v>
@@ -2246,29 +2249,29 @@
       <c r="G29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="10">
+        <v>44127</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N29" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I29" s="11">
-        <v>44127</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M29" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N29" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O29" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2276,14 +2279,14 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="18" t="s">
-        <v>114</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>134</v>
+      <c r="E30" s="14" t="s">
+        <v>133</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>23</v>
@@ -2291,29 +2294,29 @@
       <c r="G30" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="H30" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" s="10">
+        <v>44146</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M30" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N30" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I30" s="11">
-        <v>44146</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N30" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O30" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2321,15 +2324,15 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="21" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="22" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F31" s="9" t="s">
@@ -2338,29 +2341,29 @@
       <c r="G31" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I31" s="10">
+        <v>44135</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M31" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N31" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I31" s="11">
-        <v>44135</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M31" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N31" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O31" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2368,14 +2371,14 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C32" s="23"/>
+        <v>117</v>
+      </c>
+      <c r="C32" s="22"/>
       <c r="D32" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>34</v>
       </c>
       <c r="F32" s="9" t="s">
         <v>23</v>
@@ -2383,29 +2386,29 @@
       <c r="G32" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="10">
+        <v>44135</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I32" s="11">
-        <v>44135</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K32" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L32" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M32" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O32" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2413,14 +2416,14 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="23"/>
+        <v>118</v>
+      </c>
+      <c r="C33" s="22"/>
       <c r="D33" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>37</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>23</v>
@@ -2428,29 +2431,29 @@
       <c r="G33" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" s="10">
+        <v>44136</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N33" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I33" s="11">
-        <v>44136</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O33" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2458,14 +2461,14 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34" s="23"/>
+        <v>119</v>
+      </c>
+      <c r="C34" s="22"/>
       <c r="D34" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>40</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>23</v>
@@ -2473,29 +2476,29 @@
       <c r="G34" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I34" s="10">
+        <v>44135</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M34" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I34" s="11">
-        <v>44135</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N34" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O34" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2503,14 +2506,14 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>123</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>23</v>
@@ -2518,29 +2521,29 @@
       <c r="G35" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H35" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="10">
+        <v>44160</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N35" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I35" s="11">
-        <v>44160</v>
-      </c>
-      <c r="J35" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N35" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O35" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2548,14 +2551,14 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="14" t="s">
         <v>125</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>126</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>23</v>
@@ -2563,29 +2566,29 @@
       <c r="G36" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H36" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="10">
+        <v>44160</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M36" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N36" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="I36" s="11">
-        <v>44160</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K36" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M36" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N36" s="9" t="s">
-        <v>77</v>
-      </c>
       <c r="O36" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2593,14 +2596,14 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="22"/>
+      <c r="D37" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="14" t="s">
+      <c r="E37" s="14" t="s">
         <v>129</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>23</v>
@@ -2608,29 +2611,29 @@
       <c r="G37" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H37" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I37" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>45</v>
+      <c r="H37" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I37" s="10">
+        <v>44160</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M37" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2638,14 +2641,14 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="23"/>
+      <c r="D38" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C38" s="24"/>
-      <c r="D38" s="6" t="s">
+      <c r="E38" s="15" t="s">
         <v>132</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>133</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>23</v>
@@ -2653,29 +2656,29 @@
       <c r="G38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="I38" s="11">
-        <v>44155</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>45</v>
+      <c r="H38" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="I38" s="10">
+        <v>44160</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M38" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Tacna FyD: Inicio, Tacna FyD Delivery: correcion de seguimiento pedido
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46D1A3-5CC6-4610-86E3-D47725026900}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256F0823-1C72-4CDB-91C1-00CB661DD1BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,6 +717,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -734,9 +737,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -982,29 +982,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="26" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1060,7 +1060,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1107,7 +1107,7 @@
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="7" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1152,7 @@
       <c r="B5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="B7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="B8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="13" t="s">
         <v>47</v>
       </c>
@@ -1334,7 +1334,7 @@
       <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="13" t="s">
         <v>50</v>
       </c>
@@ -1379,7 +1379,7 @@
       <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
@@ -1424,7 +1424,7 @@
       <c r="B11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="13" t="s">
         <v>56</v>
       </c>
@@ -1469,7 +1469,7 @@
       <c r="B12" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="22"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="13" t="s">
         <v>61</v>
       </c>
@@ -1482,7 +1482,7 @@
       <c r="G12" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="18" t="s">
         <v>134</v>
       </c>
       <c r="I12" s="10">
@@ -1514,7 +1514,7 @@
       <c r="B13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="13" t="s">
         <v>64</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="B14" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="22"/>
+      <c r="C14" s="23"/>
       <c r="D14" s="13" t="s">
         <v>68</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="B15" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="13" t="s">
         <v>71</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="B16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="22" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1696,7 +1696,7 @@
       <c r="B17" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="22"/>
+      <c r="C17" s="23"/>
       <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1741,7 +1741,7 @@
       <c r="B18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C18" s="22"/>
+      <c r="C18" s="23"/>
       <c r="D18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1786,7 +1786,7 @@
       <c r="B19" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="22"/>
+      <c r="C19" s="23"/>
       <c r="D19" s="7" t="s">
         <v>38</v>
       </c>
@@ -1831,7 +1831,7 @@
       <c r="B20" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="22"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="7" t="s">
         <v>82</v>
       </c>
@@ -1876,7 +1876,7 @@
       <c r="B21" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="22"/>
+      <c r="C21" s="23"/>
       <c r="D21" s="7" t="s">
         <v>85</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C22" s="22"/>
+      <c r="C22" s="23"/>
       <c r="D22" s="7" t="s">
         <v>88</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="B23" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="22"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="17" t="s">
         <v>42</v>
       </c>
@@ -2011,7 +2011,7 @@
       <c r="B24" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="22"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="17" t="s">
         <v>94</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="B25" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="22"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="7" t="s">
         <v>97</v>
       </c>
@@ -2101,7 +2101,7 @@
       <c r="B26" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="22"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="17" t="s">
         <v>100</v>
       </c>
@@ -2146,7 +2146,7 @@
       <c r="B27" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C27" s="22"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="17" t="s">
         <v>103</v>
       </c>
@@ -2191,7 +2191,7 @@
       <c r="B28" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C28" s="22"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="17" t="s">
         <v>106</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="B29" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="22"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="17" t="s">
         <v>110</v>
       </c>
@@ -2281,7 +2281,7 @@
       <c r="B30" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="17" t="s">
         <v>113</v>
       </c>
@@ -2326,7 +2326,7 @@
       <c r="B31" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="22" t="s">
         <v>115</v>
       </c>
       <c r="D31" s="7" t="s">
@@ -2373,7 +2373,7 @@
       <c r="B32" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="22"/>
+      <c r="C32" s="23"/>
       <c r="D32" s="7" t="s">
         <v>32</v>
       </c>
@@ -2418,7 +2418,7 @@
       <c r="B33" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="22"/>
+      <c r="C33" s="23"/>
       <c r="D33" s="7" t="s">
         <v>35</v>
       </c>
@@ -2463,7 +2463,7 @@
       <c r="B34" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="22"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="7" t="s">
         <v>38</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="B35" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C35" s="22"/>
+      <c r="C35" s="23"/>
       <c r="D35" s="7" t="s">
         <v>121</v>
       </c>
@@ -2553,7 +2553,7 @@
       <c r="B36" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="22"/>
+      <c r="C36" s="23"/>
       <c r="D36" s="13" t="s">
         <v>113</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="B37" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C37" s="22"/>
+      <c r="C37" s="23"/>
       <c r="D37" s="13" t="s">
         <v>128</v>
       </c>
@@ -2643,7 +2643,7 @@
       <c r="B38" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C38" s="23"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="6" t="s">
         <v>131</v>
       </c>
@@ -2656,11 +2656,11 @@
       <c r="G38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="27" t="s">
-        <v>134</v>
+      <c r="H38" s="16" t="s">
+        <v>75</v>
       </c>
       <c r="I38" s="10">
-        <v>44160</v>
+        <v>44172</v>
       </c>
       <c r="J38" s="11" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Actualización de documentos, definición de requerimientos
Actualización de documentos, definición de requerimientos
</commit_message>
<xml_diff>
--- a/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
+++ b/Documentos/3. Elaboracion/Matriz de trazabilidad_Ordoñez_Rivas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPT\Construccion II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ademuz\Documents\GitHub\Tacna-FD-Construccion-II\Tacna-FD-Construccion-II\Documentos\3. Elaboracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8D3021-4500-43A7-A0F9-FE439034ECDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777622DF-641C-490F-9BC6-8DF773823F8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16635" yWindow="2430" windowWidth="17280" windowHeight="9105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -198,9 +198,6 @@
     <t>Obtener Vale</t>
   </si>
   <si>
-    <t>La aplicación debe permitir la obtención de un vale o cupón de descuento al realizar un numero especifico de reseñas.</t>
-  </si>
-  <si>
     <t>v2</t>
   </si>
   <si>
@@ -213,18 +210,12 @@
     <t>Listar Vale</t>
   </si>
   <si>
-    <t>La aplicación debe permitir al usuario visualizar en la pantalla sus vales obtenidos y se eliminaran una vez haya sido usados.</t>
-  </si>
-  <si>
     <t>RF-11</t>
   </si>
   <si>
     <t>Realizar Pedido</t>
   </si>
   <si>
-    <t>La aplicación debe permitir al usuario seleccionar los ítems que desea comprar del menú del establecimiento, así como también indicar la cantidad de estos, y también poder permitir al cliente elegir el método de envió, además debe permitir el pago respectivo a través de PayPal, tarjetas de crédito o débito, o pago contra entrega por medio de Yape, Tunki o Lukita</t>
-  </si>
-  <si>
     <t>Modulo Pedidos (Tacna F&amp;D)</t>
   </si>
   <si>
@@ -427,13 +418,24 @@
   </si>
   <si>
     <t>La aplicación debe permitir que el usuario pueda visualizar todos los pedidos (pendiente, en camino, entregado o separado) realizados por los clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">La aplicación debe permitir la obtención de un vale o cupón de descuento al realizar un número de 5 reseñas.
+La aplicación también debe permitir al usuario visualizar en la parte inferior de la pantalla la lista de sus vales obtenidos y se podrá visualizar su detalle al ser seleccionado y la opción de utilizar el cupón...
+</t>
+  </si>
+  <si>
+    <t>La aplicación debe permitir que los usuarios puedan visualizar los cupones de cada establecimiento.</t>
+  </si>
+  <si>
+    <t>La aplicación debe permitir seleccionar la ubicación destino de la entrega y rellenar automáticamente su dirección, además de poder editarla. Podrá seleccionar los ítems del menú que desea comprar del establecimiento, así como también indicar la cantidad de estos, y además el usuario podrá visualizar los datos del pedido y permitir elegir el método de envió por recojo en tienda o delivery...</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +474,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -648,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -700,6 +708,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -937,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -962,29 +973,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="26" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="20"/>
-      <c r="M1" s="18" t="s">
+      <c r="L1" s="21"/>
+      <c r="M1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1040,7 +1051,7 @@
       <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -1056,7 +1067,7 @@
         <v>24</v>
       </c>
       <c r="H3" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I3" s="10">
         <v>44135</v>
@@ -1087,7 +1098,7 @@
       <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="7" t="s">
         <v>32</v>
       </c>
@@ -1101,7 +1112,7 @@
         <v>24</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I4" s="10">
         <v>44135</v>
@@ -1132,7 +1143,7 @@
       <c r="B5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="7" t="s">
         <v>35</v>
       </c>
@@ -1146,7 +1157,7 @@
         <v>24</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I5" s="10">
         <v>44140</v>
@@ -1178,7 +1189,7 @@
       <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="7" t="s">
         <v>38</v>
       </c>
@@ -1192,7 +1203,7 @@
         <v>24</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I6" s="10">
         <v>44135</v>
@@ -1224,7 +1235,7 @@
       <c r="B7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="7" t="s">
         <v>42</v>
       </c>
@@ -1238,7 +1249,7 @@
         <v>24</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I7" s="10">
         <v>44143</v>
@@ -1269,7 +1280,7 @@
       <c r="B8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="13" t="s">
         <v>47</v>
       </c>
@@ -1283,7 +1294,7 @@
         <v>24</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I8" s="10">
         <v>44147</v>
@@ -1314,7 +1325,7 @@
       <c r="B9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="22"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="13" t="s">
         <v>50</v>
       </c>
@@ -1328,7 +1339,7 @@
         <v>24</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I9" s="10">
         <v>44147</v>
@@ -1359,7 +1370,7 @@
       <c r="B10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="13" t="s">
         <v>53</v>
       </c>
@@ -1373,7 +1384,7 @@
         <v>24</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I10" s="10">
         <v>44146</v>
@@ -1397,31 +1408,31 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="214.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="13" t="s">
         <v>56</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I11" s="10">
-        <v>44155</v>
+        <v>44184</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>44</v>
@@ -1439,7 +1450,7 @@
         <v>29</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1447,26 +1458,26 @@
         <v>10</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="E12" s="14" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I12" s="10">
-        <v>44178</v>
+        <v>44152</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>44</v>
@@ -1484,7 +1495,7 @@
         <v>29</v>
       </c>
       <c r="O12" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="228" customHeight="1" x14ac:dyDescent="0.2">
@@ -1492,26 +1503,26 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="22"/>
+        <v>61</v>
+      </c>
+      <c r="C13" s="23"/>
       <c r="D13" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>133</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H13" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I13" s="10">
-        <v>44152</v>
+        <v>44184</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>44</v>
@@ -1529,7 +1540,7 @@
         <v>29</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1537,14 +1548,14 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="22"/>
+        <v>64</v>
+      </c>
+      <c r="C14" s="23"/>
       <c r="D14" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>23</v>
@@ -1553,7 +1564,7 @@
         <v>24</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I14" s="10">
         <v>44153</v>
@@ -1574,7 +1585,7 @@
         <v>29</v>
       </c>
       <c r="O14" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="89.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,14 +1593,14 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="23"/>
+        <v>67</v>
+      </c>
+      <c r="C15" s="24"/>
       <c r="D15" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F15" s="9" t="s">
         <v>23</v>
@@ -1598,7 +1609,7 @@
         <v>24</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I15" s="10">
         <v>44160</v>
@@ -1619,7 +1630,7 @@
         <v>29</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="84" customHeight="1" x14ac:dyDescent="0.2">
@@ -1627,10 +1638,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>21</v>
@@ -1645,7 +1656,7 @@
         <v>24</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I16" s="10">
         <v>44109</v>
@@ -1663,10 +1674,10 @@
         <v>28</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O16" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1674,9 +1685,9 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="22"/>
+        <v>75</v>
+      </c>
+      <c r="C17" s="23"/>
       <c r="D17" s="7" t="s">
         <v>32</v>
       </c>
@@ -1690,7 +1701,7 @@
         <v>24</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I17" s="10">
         <v>44109</v>
@@ -1708,10 +1719,10 @@
         <v>28</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1719,9 +1730,9 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" s="22"/>
+        <v>76</v>
+      </c>
+      <c r="C18" s="23"/>
       <c r="D18" s="7" t="s">
         <v>35</v>
       </c>
@@ -1735,7 +1746,7 @@
         <v>24</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I18" s="10">
         <v>44112</v>
@@ -1753,10 +1764,10 @@
         <v>28</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="132" customHeight="1" x14ac:dyDescent="0.2">
@@ -1764,9 +1775,9 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="22"/>
+        <v>77</v>
+      </c>
+      <c r="C19" s="23"/>
       <c r="D19" s="7" t="s">
         <v>38</v>
       </c>
@@ -1780,7 +1791,7 @@
         <v>24</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I19" s="10">
         <v>44109</v>
@@ -1798,10 +1809,10 @@
         <v>28</v>
       </c>
       <c r="N19" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O19" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="165" customHeight="1" x14ac:dyDescent="0.2">
@@ -1809,14 +1820,14 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="22"/>
+        <v>78</v>
+      </c>
+      <c r="C20" s="23"/>
       <c r="D20" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F20" s="9" t="s">
         <v>23</v>
@@ -1825,7 +1836,7 @@
         <v>24</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I20" s="10">
         <v>44131</v>
@@ -1843,10 +1854,10 @@
         <v>28</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="257.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1854,14 +1865,14 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21" s="22"/>
+        <v>81</v>
+      </c>
+      <c r="C21" s="23"/>
       <c r="D21" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F21" s="9" t="s">
         <v>23</v>
@@ -1870,7 +1881,7 @@
         <v>24</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I21" s="10">
         <v>44132</v>
@@ -1888,10 +1899,10 @@
         <v>28</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1899,14 +1910,14 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="22"/>
+        <v>84</v>
+      </c>
+      <c r="C22" s="23"/>
       <c r="D22" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F22" s="9" t="s">
         <v>23</v>
@@ -1915,7 +1926,7 @@
         <v>24</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I22" s="10">
         <v>44117</v>
@@ -1933,10 +1944,10 @@
         <v>28</v>
       </c>
       <c r="N22" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1944,14 +1955,14 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C23" s="22"/>
+        <v>88</v>
+      </c>
+      <c r="C23" s="23"/>
       <c r="D23" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>23</v>
@@ -1960,7 +1971,7 @@
         <v>24</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I23" s="10">
         <v>44117</v>
@@ -1978,10 +1989,10 @@
         <v>28</v>
       </c>
       <c r="N23" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1989,14 +2000,14 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C24" s="22"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="23"/>
       <c r="D24" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>23</v>
@@ -2005,7 +2016,7 @@
         <v>24</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I24" s="10">
         <v>44122</v>
@@ -2023,10 +2034,10 @@
         <v>28</v>
       </c>
       <c r="N24" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O24" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2034,14 +2045,14 @@
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="22"/>
+        <v>93</v>
+      </c>
+      <c r="C25" s="23"/>
       <c r="D25" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>23</v>
@@ -2050,7 +2061,7 @@
         <v>24</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I25" s="10">
         <v>44127</v>
@@ -2068,10 +2079,10 @@
         <v>28</v>
       </c>
       <c r="N25" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="171" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,14 +2090,14 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="22"/>
+        <v>96</v>
+      </c>
+      <c r="C26" s="23"/>
       <c r="D26" s="17" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>23</v>
@@ -2095,7 +2106,7 @@
         <v>24</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I26" s="10">
         <v>44129</v>
@@ -2113,10 +2124,10 @@
         <v>28</v>
       </c>
       <c r="N26" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="132.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2124,14 +2135,14 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C27" s="22"/>
+        <v>99</v>
+      </c>
+      <c r="C27" s="23"/>
       <c r="D27" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>23</v>
@@ -2140,7 +2151,7 @@
         <v>24</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I27" s="10">
         <v>44128</v>
@@ -2158,10 +2169,10 @@
         <v>28</v>
       </c>
       <c r="N27" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="135" customHeight="1" x14ac:dyDescent="0.2">
@@ -2169,14 +2180,14 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C28" s="22"/>
+        <v>102</v>
+      </c>
+      <c r="C28" s="23"/>
       <c r="D28" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F28" s="9" t="s">
         <v>23</v>
@@ -2185,7 +2196,7 @@
         <v>24</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I28" s="10">
         <v>44129</v>
@@ -2203,10 +2214,10 @@
         <v>28</v>
       </c>
       <c r="N28" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O28" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="112.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2214,14 +2225,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" s="22"/>
+        <v>106</v>
+      </c>
+      <c r="C29" s="23"/>
       <c r="D29" s="17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>23</v>
@@ -2230,7 +2241,7 @@
         <v>24</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I29" s="10">
         <v>44127</v>
@@ -2248,10 +2259,10 @@
         <v>28</v>
       </c>
       <c r="N29" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2259,14 +2270,14 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C30" s="23"/>
+        <v>109</v>
+      </c>
+      <c r="C30" s="24"/>
       <c r="D30" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>23</v>
@@ -2275,7 +2286,7 @@
         <v>24</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I30" s="10">
         <v>44146</v>
@@ -2293,10 +2304,10 @@
         <v>28</v>
       </c>
       <c r="N30" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2304,10 +2315,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>115</v>
+        <v>111</v>
+      </c>
+      <c r="C31" s="22" t="s">
+        <v>112</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>21</v>
@@ -2322,7 +2333,7 @@
         <v>24</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I31" s="10">
         <v>44135</v>
@@ -2340,10 +2351,10 @@
         <v>28</v>
       </c>
       <c r="N31" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O31" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2351,9 +2362,9 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C32" s="22"/>
+        <v>114</v>
+      </c>
+      <c r="C32" s="23"/>
       <c r="D32" s="7" t="s">
         <v>32</v>
       </c>
@@ -2367,7 +2378,7 @@
         <v>24</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I32" s="10">
         <v>44135</v>
@@ -2385,10 +2396,10 @@
         <v>28</v>
       </c>
       <c r="N32" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2396,9 +2407,9 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C33" s="22"/>
+        <v>115</v>
+      </c>
+      <c r="C33" s="23"/>
       <c r="D33" s="7" t="s">
         <v>35</v>
       </c>
@@ -2412,7 +2423,7 @@
         <v>24</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I33" s="10">
         <v>44136</v>
@@ -2430,10 +2441,10 @@
         <v>28</v>
       </c>
       <c r="N33" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="161.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2441,9 +2452,9 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="22"/>
+        <v>116</v>
+      </c>
+      <c r="C34" s="23"/>
       <c r="D34" s="7" t="s">
         <v>38</v>
       </c>
@@ -2457,7 +2468,7 @@
         <v>24</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I34" s="10">
         <v>44135</v>
@@ -2475,10 +2486,10 @@
         <v>28</v>
       </c>
       <c r="N34" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2486,14 +2497,14 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C35" s="22"/>
+        <v>117</v>
+      </c>
+      <c r="C35" s="23"/>
       <c r="D35" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>23</v>
@@ -2502,7 +2513,7 @@
         <v>24</v>
       </c>
       <c r="H35" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I35" s="10">
         <v>44160</v>
@@ -2520,10 +2531,10 @@
         <v>28</v>
       </c>
       <c r="N35" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O35" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2531,14 +2542,14 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C36" s="22"/>
+        <v>121</v>
+      </c>
+      <c r="C36" s="23"/>
       <c r="D36" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F36" s="9" t="s">
         <v>23</v>
@@ -2547,7 +2558,7 @@
         <v>24</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I36" s="10">
         <v>44160</v>
@@ -2565,10 +2576,10 @@
         <v>28</v>
       </c>
       <c r="N36" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O36" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2576,14 +2587,14 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C37" s="22"/>
+        <v>124</v>
+      </c>
+      <c r="C37" s="23"/>
       <c r="D37" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>23</v>
@@ -2592,7 +2603,7 @@
         <v>24</v>
       </c>
       <c r="H37" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I37" s="10">
         <v>44160</v>
@@ -2610,10 +2621,10 @@
         <v>28</v>
       </c>
       <c r="N37" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O37" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2621,14 +2632,14 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C38" s="23"/>
+        <v>127</v>
+      </c>
+      <c r="C38" s="24"/>
       <c r="D38" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>23</v>
@@ -2637,7 +2648,7 @@
         <v>24</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I38" s="10">
         <v>44172</v>
@@ -2655,10 +2666,10 @@
         <v>28</v>
       </c>
       <c r="N38" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="O38" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>